<commit_message>
working buttons and basic screens
</commit_message>
<xml_diff>
--- a/workspace/bluepill-proto/ADC_Conversions.xlsx
+++ b/workspace/bluepill-proto/ADC_Conversions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Documents\Git\RT_soldering_pen\workspace\bluepill-proto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F231C016-C7F4-40CF-B50B-4FA7A9C2FB2C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B676DE33-D10D-417F-914B-46D127245B60}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="3405" windowWidth="29040" windowHeight="15990" xr2:uid="{95DD0E50-A309-4C4B-A38C-D139287163B0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{95DD0E50-A309-4C4B-A38C-D139287163B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="22">
   <si>
     <t>Overrun limits</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t>convertTipTemp(1/10C)</t>
+  </si>
+  <si>
+    <t>80C</t>
+  </si>
+  <si>
+    <t>190C</t>
+  </si>
+  <si>
+    <t>500-25</t>
   </si>
 </sst>
 </file>
@@ -468,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3872F1FC-7226-42BE-A34E-40A3ADD96BA6}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1396,7 +1405,7 @@
         <v>33000</v>
       </c>
       <c r="E27">
-        <f t="shared" ref="E27:E28" si="25">ROUND(D27*C27, 0)</f>
+        <f t="shared" ref="E27" si="25">ROUND(D27*C27, 0)</f>
         <v>491502000</v>
       </c>
       <c r="F27" s="1">
@@ -1538,18 +1547,18 @@
         <v>13116414</v>
       </c>
       <c r="H31" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="I31">
         <f>ROUND(H31*G31, 0)</f>
-        <v>1311641400</v>
+        <v>131164140</v>
       </c>
       <c r="J31" s="1">
         <v>65535</v>
       </c>
       <c r="K31">
-        <f>I31/J31</f>
-        <v>20014.364843213549</v>
+        <f>ROUND(I31/J31, 0)</f>
+        <v>2001</v>
       </c>
       <c r="O31" t="s">
         <v>1</v>
@@ -1581,18 +1590,18 @@
         <v>6558316</v>
       </c>
       <c r="H32" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="I32">
         <f t="shared" ref="I32:I33" si="30">ROUND(H32*G32, 0)</f>
-        <v>655831600</v>
+        <v>65583160</v>
       </c>
       <c r="J32" s="1">
         <v>65535</v>
       </c>
       <c r="K32">
-        <f t="shared" ref="K32:K33" si="31">I32/J32</f>
-        <v>10007.34874494545</v>
+        <f t="shared" ref="K32:K33" si="31">ROUND(I32/J32, 0)</f>
+        <v>1001</v>
       </c>
       <c r="O32" t="s">
         <v>2</v>
@@ -1621,21 +1630,40 @@
         <v>1689263</v>
       </c>
       <c r="H33" s="1">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="I33">
         <f t="shared" si="30"/>
-        <v>168926300</v>
+        <v>16892630</v>
       </c>
       <c r="J33" s="1">
         <v>65535</v>
       </c>
       <c r="K33">
         <f t="shared" si="31"/>
-        <v>2577.6501106279088</v>
+        <v>258</v>
       </c>
       <c r="O33" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B39">
+        <f>80-25</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>